<commit_message>
Added BAARD stage 2,  line, watermark to CIFAR10
</commit_message>
<xml_diff>
--- a/tables/banknote_basic16_5.xlsx
+++ b/tables/banknote_basic16_5.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -691,19 +691,19 @@
         </is>
       </c>
       <c r="B8" s="1" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="C8" t="n">
-        <v>68.87755102040815</v>
+        <v>91.32653061224491</v>
       </c>
       <c r="D8" t="n">
-        <v>69.38775510204081</v>
+        <v>91.32653061224491</v>
       </c>
       <c r="E8" t="n">
-        <v>39.28571428571428</v>
+        <v>91.32653061224491</v>
       </c>
       <c r="F8" t="n">
-        <v>9.183673469387756</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
         <v>2.040816326530612</v>
@@ -712,7 +712,7 @@
         <v>2.040816326530612</v>
       </c>
       <c r="I8" t="n">
-        <v>6.632653061224491</v>
+        <v>1.020408163265306</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
@@ -721,19 +721,19 @@
     <row r="9">
       <c r="A9" s="1" t="n"/>
       <c r="B9" s="1" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>91.32653061224491</v>
+        <v>100</v>
       </c>
       <c r="D9" t="n">
-        <v>91.32653061224491</v>
+        <v>100</v>
       </c>
       <c r="E9" t="n">
-        <v>91.32653061224491</v>
+        <v>100</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>0.5102040816326531</v>
       </c>
       <c r="G9" t="n">
         <v>2.040816326530612</v>
@@ -742,7 +742,7 @@
         <v>2.040816326530612</v>
       </c>
       <c r="I9" t="n">
-        <v>1.020408163265306</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
@@ -751,7 +751,7 @@
     <row r="10">
       <c r="A10" s="1" t="n"/>
       <c r="B10" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
         <v>100</v>
@@ -760,10 +760,10 @@
         <v>100</v>
       </c>
       <c r="E10" t="n">
-        <v>100</v>
+        <v>96.93877551020408</v>
       </c>
       <c r="F10" t="n">
-        <v>0.5102040816326531</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
         <v>2.040816326530612</v>
@@ -781,7 +781,7 @@
     <row r="11">
       <c r="A11" s="1" t="n"/>
       <c r="B11" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" t="n">
         <v>100</v>
@@ -790,7 +790,7 @@
         <v>100</v>
       </c>
       <c r="E11" t="n">
-        <v>96.93877551020408</v>
+        <v>100</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -809,21 +809,25 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n"/>
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>boundary</t>
+        </is>
+      </c>
       <c r="B12" s="1" t="n">
-        <v>3</v>
+        <v>0.3</v>
       </c>
       <c r="C12" t="n">
-        <v>100</v>
+        <v>88.77551020408163</v>
       </c>
       <c r="D12" t="n">
-        <v>100</v>
+        <v>91.32653061224491</v>
       </c>
       <c r="E12" t="n">
-        <v>100</v>
+        <v>75.51020408163265</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>50.51020408163265</v>
       </c>
       <c r="G12" t="n">
         <v>2.040816326530612</v>
@@ -832,7 +836,7 @@
         <v>2.040816326530612</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>5.612244897959183</v>
       </c>
       <c r="J12" t="n">
         <v>0</v>
@@ -841,23 +845,23 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>boundary</t>
+          <t>cw2</t>
         </is>
       </c>
       <c r="B13" s="1" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>88.77551020408163</v>
+        <v>77.55102040816327</v>
       </c>
       <c r="D13" t="n">
-        <v>91.32653061224491</v>
+        <v>83.16326530612244</v>
       </c>
       <c r="E13" t="n">
-        <v>75.51020408163265</v>
+        <v>63.26530612244898</v>
       </c>
       <c r="F13" t="n">
-        <v>50.51020408163265</v>
+        <v>55.10204081632652</v>
       </c>
       <c r="G13" t="n">
         <v>2.040816326530612</v>
@@ -873,25 +877,21 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>cw2</t>
-        </is>
-      </c>
+      <c r="A14" s="1" t="n"/>
       <c r="B14" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C14" t="n">
-        <v>77.55102040816327</v>
+        <v>56.63265306122449</v>
       </c>
       <c r="D14" t="n">
-        <v>83.16326530612244</v>
+        <v>59.18367346938776</v>
       </c>
       <c r="E14" t="n">
-        <v>63.26530612244898</v>
+        <v>34.18367346938776</v>
       </c>
       <c r="F14" t="n">
-        <v>55.10204081632652</v>
+        <v>1.020408163265306</v>
       </c>
       <c r="G14" t="n">
         <v>2.040816326530612</v>
@@ -900,7 +900,7 @@
         <v>2.040816326530612</v>
       </c>
       <c r="I14" t="n">
-        <v>5.612244897959183</v>
+        <v>9.693877551020408</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
@@ -909,16 +909,16 @@
     <row r="15">
       <c r="A15" s="1" t="n"/>
       <c r="B15" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C15" t="n">
-        <v>56.63265306122449</v>
+        <v>89.79591836734693</v>
       </c>
       <c r="D15" t="n">
-        <v>59.18367346938776</v>
+        <v>89.79591836734693</v>
       </c>
       <c r="E15" t="n">
-        <v>34.18367346938776</v>
+        <v>79.59183673469387</v>
       </c>
       <c r="F15" t="n">
         <v>1.020408163265306</v>
@@ -930,37 +930,41 @@
         <v>2.040816326530612</v>
       </c>
       <c r="I15" t="n">
-        <v>9.693877551020408</v>
+        <v>1.020408163265306</v>
       </c>
       <c r="J15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n"/>
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>deepfool</t>
+        </is>
+      </c>
       <c r="B16" s="1" t="n">
-        <v>10</v>
+        <v>1e-06</v>
       </c>
       <c r="C16" t="n">
-        <v>89.79591836734693</v>
+        <v>94.89795918367348</v>
       </c>
       <c r="D16" t="n">
-        <v>89.79591836734693</v>
+        <v>96.42857142857143</v>
       </c>
       <c r="E16" t="n">
-        <v>79.59183673469387</v>
+        <v>87.75510204081633</v>
       </c>
       <c r="F16" t="n">
-        <v>1.020408163265306</v>
+        <v>1.530612244897959</v>
       </c>
       <c r="G16" t="n">
-        <v>2.040816326530612</v>
+        <v>3.061224489795918</v>
       </c>
       <c r="H16" t="n">
-        <v>2.040816326530612</v>
+        <v>5.612244897959183</v>
       </c>
       <c r="I16" t="n">
-        <v>1.020408163265306</v>
+        <v>0.5102040816326531</v>
       </c>
       <c r="J16" t="n">
         <v>0</v>
@@ -969,57 +973,53 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>deepfool</t>
+          <t>fgsm</t>
         </is>
       </c>
       <c r="B17" s="1" t="n">
-        <v>1e-06</v>
+        <v>0.05</v>
       </c>
       <c r="C17" t="n">
+        <v>96.42857142857143</v>
+      </c>
+      <c r="D17" t="n">
+        <v>98.46938775510205</v>
+      </c>
+      <c r="E17" t="n">
+        <v>92.3469387755102</v>
+      </c>
+      <c r="F17" t="n">
+        <v>76.0204081632653</v>
+      </c>
+      <c r="G17" t="n">
+        <v>2.040816326530612</v>
+      </c>
+      <c r="H17" t="n">
+        <v>2.040816326530612</v>
+      </c>
+      <c r="I17" t="n">
+        <v>5.102040816326531</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n"/>
+      <c r="B18" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C18" t="n">
         <v>94.89795918367348</v>
       </c>
-      <c r="D17" t="n">
-        <v>96.42857142857143</v>
-      </c>
-      <c r="E17" t="n">
-        <v>87.75510204081633</v>
-      </c>
-      <c r="F17" t="n">
-        <v>1.530612244897959</v>
-      </c>
-      <c r="G17" t="n">
-        <v>3.061224489795918</v>
-      </c>
-      <c r="H17" t="n">
-        <v>5.612244897959183</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0.5102040816326531</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>fgsm</t>
-        </is>
-      </c>
-      <c r="B18" s="1" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="C18" t="n">
-        <v>96.42857142857143</v>
-      </c>
       <c r="D18" t="n">
-        <v>98.46938775510205</v>
+        <v>94.89795918367348</v>
       </c>
       <c r="E18" t="n">
-        <v>92.3469387755102</v>
+        <v>78.57142857142857</v>
       </c>
       <c r="F18" t="n">
-        <v>76.0204081632653</v>
+        <v>1.020408163265306</v>
       </c>
       <c r="G18" t="n">
         <v>2.040816326530612</v>
@@ -1028,7 +1028,7 @@
         <v>2.040816326530612</v>
       </c>
       <c r="I18" t="n">
-        <v>5.102040816326531</v>
+        <v>4.591836734693878</v>
       </c>
       <c r="J18" t="n">
         <v>0</v>
@@ -1037,28 +1037,28 @@
     <row r="19">
       <c r="A19" s="1" t="n"/>
       <c r="B19" s="1" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="C19" t="n">
-        <v>94.89795918367348</v>
+        <v>100</v>
       </c>
       <c r="D19" t="n">
-        <v>94.89795918367348</v>
+        <v>100</v>
       </c>
       <c r="E19" t="n">
-        <v>78.57142857142857</v>
+        <v>98.46938775510205</v>
       </c>
       <c r="F19" t="n">
-        <v>1.020408163265306</v>
+        <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>2.040816326530612</v>
+        <v>2.551020408163265</v>
       </c>
       <c r="H19" t="n">
         <v>2.040816326530612</v>
       </c>
       <c r="I19" t="n">
-        <v>4.591836734693878</v>
+        <v>0</v>
       </c>
       <c r="J19" t="n">
         <v>0</v>
@@ -1067,7 +1067,7 @@
     <row r="20">
       <c r="A20" s="1" t="n"/>
       <c r="B20" s="1" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="C20" t="n">
         <v>100</v>
@@ -1076,13 +1076,13 @@
         <v>100</v>
       </c>
       <c r="E20" t="n">
-        <v>98.46938775510205</v>
+        <v>97.44897959183672</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>2.551020408163265</v>
+        <v>2.040816326530612</v>
       </c>
       <c r="H20" t="n">
         <v>2.040816326530612</v>
@@ -1091,36 +1091,6 @@
         <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n"/>
-      <c r="B21" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" t="n">
-        <v>100</v>
-      </c>
-      <c r="D21" t="n">
-        <v>100</v>
-      </c>
-      <c r="E21" t="n">
-        <v>97.44897959183672</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0</v>
-      </c>
-      <c r="G21" t="n">
-        <v>2.040816326530612</v>
-      </c>
-      <c r="H21" t="n">
-        <v>2.040816326530612</v>
-      </c>
-      <c r="I21" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1129,9 +1099,9 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A17:A20"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
BAARD  uses fixed training set
</commit_message>
<xml_diff>
--- a/tables/banknote_basic16_5.xlsx
+++ b/tables/banknote_basic16_5.xlsx
@@ -579,7 +579,7 @@
         <v>92.85714285714286</v>
       </c>
       <c r="F4" t="n">
-        <v>79.59183673469387</v>
+        <v>78.57142857142857</v>
       </c>
       <c r="G4" t="n">
         <v>3.061224489795918</v>
@@ -600,7 +600,7 @@
         <v>0.2</v>
       </c>
       <c r="C5" t="n">
-        <v>96.93877551020408</v>
+        <v>94.3877551020408</v>
       </c>
       <c r="D5" t="n">
         <v>95.40816326530613</v>
@@ -821,7 +821,7 @@
         <v>88.77551020408163</v>
       </c>
       <c r="D12" t="n">
-        <v>91.32653061224491</v>
+        <v>91.83673469387756</v>
       </c>
       <c r="E12" t="n">
         <v>75.51020408163265</v>
@@ -852,7 +852,7 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>77.55102040816327</v>
+        <v>79.08163265306123</v>
       </c>
       <c r="D13" t="n">
         <v>83.16326530612244</v>
@@ -885,7 +885,7 @@
         <v>56.63265306122449</v>
       </c>
       <c r="D14" t="n">
-        <v>59.18367346938776</v>
+        <v>56.63265306122449</v>
       </c>
       <c r="E14" t="n">
         <v>34.18367346938776</v>
@@ -1052,7 +1052,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>2.551020408163265</v>
+        <v>2.040816326530612</v>
       </c>
       <c r="H19" t="n">
         <v>2.040816326530612</v>

</xml_diff>